<commit_message>
Added Aprovecho pictures, and all of the tex files for lab report 1.  Made a few python programs to get all of the lab report data.
</commit_message>
<xml_diff>
--- a/ME552/Lab 1/Lab_1_Dimensions(1).xlsx
+++ b/ME552/Lab 1/Lab_1_Dimensions(1).xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Windows.Documents\My Documents\GS Files\Research\TAship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewalferman/Desktop/Classes/ME552/Lab 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -90,91 +96,91 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,17 +483,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +508,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -519,7 +525,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="E4">
@@ -532,7 +538,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -547,7 +553,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -564,7 +570,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -581,7 +587,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
@@ -599,7 +605,7 @@
         <v>0.12479999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>5</v>
       </c>

</xml_diff>